<commit_message>
update data and notebooks
</commit_message>
<xml_diff>
--- a/data/data_dict.xlsx
+++ b/data/data_dict.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyayut.chi\Documents\github\price_transmission\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A33DC5-6A79-42A2-89AB-7F4506983F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C944C2-21D0-4620-BC82-FCAF5C266059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="rice" sheetId="1" r:id="rId1"/>
+    <sheet name="bran" sheetId="7" r:id="rId1"/>
+    <sheet name="e" sheetId="6" r:id="rId2"/>
+    <sheet name="d" sheetId="5" r:id="rId3"/>
+    <sheet name="cc" sheetId="4" r:id="rId4"/>
+    <sheet name="bb" sheetId="3" r:id="rId5"/>
+    <sheet name="aa" sheetId="2" r:id="rId6"/>
+    <sheet name="rice" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">rice!$A$1:$K$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">rice!$A$1:$K$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="149">
   <si>
     <t>RH</t>
   </si>
@@ -507,6 +513,78 @@
   <si>
     <t>รำข้าว</t>
   </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>aa_name</t>
+  </si>
+  <si>
+    <t>aa_name_th</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>bb_name</t>
+  </si>
+  <si>
+    <t>bb_name_th</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>cc_name</t>
+  </si>
+  <si>
+    <t>cc_name_th</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>d_name</t>
+  </si>
+  <si>
+    <t>d_name_th</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>e_name</t>
+  </si>
+  <si>
+    <t>e_name_th</t>
+  </si>
+  <si>
+    <t>bran</t>
+  </si>
+  <si>
+    <t>bran_name</t>
+  </si>
+  <si>
+    <t>bran_name_th</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>35%</t>
+  </si>
+  <si>
+    <t>45%</t>
+  </si>
+  <si>
+    <t>ZZ</t>
+  </si>
 </sst>
 </file>
 
@@ -562,7 +640,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +659,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -594,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -606,6 +690,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,13 +970,695 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43E12BB-F007-4932-843D-4497124A8855}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FA77BE-AE2A-4688-8D46-CF284338D445}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A7" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FA36E8-BA29-4844-B35F-ED75A7E5479E}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A12" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5778AD6-63D4-4D41-A106-E2EDD046EDEE}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A1" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A13" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A39B4C-611C-4B5A-9B7A-72D58AAEAE7C}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A1" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3D403C-6855-44B6-A25A-2C8BF99361EA}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A1" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.7">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="E5:G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" x14ac:dyDescent="0.7"/>
   <cols>
@@ -1155,13 +1922,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.7">
       <c r="E11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>144</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>82</v>
@@ -1179,14 +1946,14 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="E12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>75</v>
+      <c r="E12" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>27</v>
@@ -1208,14 +1975,14 @@
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>90</v>
+      <c r="E13" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>63</v>
@@ -1237,6 +2004,15 @@
       <c r="C14" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="I14" s="4" t="s">
         <v>107</v>
       </c>
@@ -1257,11 +2033,15 @@
       <c r="C15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="E15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A16" s="4" t="s">
@@ -1273,15 +2053,6 @@
       <c r="C16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="I16" s="6" t="s">
         <v>124</v>
       </c>
@@ -1298,15 +2069,11 @@
       <c r="C17" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="E17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
       <c r="I17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1327,14 +2094,14 @@
       <c r="C18" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>35</v>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>99</v>
@@ -1357,13 +2124,13 @@
         <v>119</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>101</v>
@@ -1385,14 +2152,14 @@
       <c r="C20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>81</v>
+      <c r="E20" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>102</v>
@@ -1405,14 +2172,14 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.7">
-      <c r="E21" s="1" t="s">
-        <v>27</v>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>103</v>
@@ -1422,6 +2189,28 @@
       </c>
       <c r="K21" s="1" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="E22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.7">
+      <c r="E23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>